<commit_message>
Formateo código y organización y lineas tendencia
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -470,16 +470,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="C2" t="n">
-        <v>238</v>
+        <v>162</v>
       </c>
       <c r="D2" t="n">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="E2" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -493,22 +493,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>163</v>
+        <v>232</v>
       </c>
       <c r="C3" t="n">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D3" t="n">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="E3" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="F3" t="n">
-        <v>23400</v>
+        <v>27000</v>
       </c>
       <c r="G3" t="n">
-        <v>49500</v>
+        <v>46000</v>
       </c>
     </row>
     <row r="4">
@@ -516,22 +516,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C4" t="n">
-        <v>201</v>
+        <v>230</v>
       </c>
       <c r="D4" t="n">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="E4" t="n">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="F4" t="n">
-        <v>24000</v>
+        <v>28536</v>
       </c>
       <c r="G4" t="n">
-        <v>52622</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="5">
@@ -539,22 +539,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>115</v>
+        <v>233</v>
       </c>
       <c r="C5" t="n">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="D5" t="n">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="E5" t="n">
-        <v>280</v>
+        <v>211</v>
       </c>
       <c r="F5" t="n">
-        <v>22841</v>
+        <v>29670</v>
       </c>
       <c r="G5" t="n">
-        <v>56000</v>
+        <v>46631</v>
       </c>
     </row>
     <row r="6">
@@ -562,22 +562,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="C6" t="n">
-        <v>104</v>
+        <v>178</v>
       </c>
       <c r="D6" t="n">
-        <v>216</v>
+        <v>137</v>
       </c>
       <c r="E6" t="n">
-        <v>315</v>
+        <v>213</v>
       </c>
       <c r="F6" t="n">
-        <v>24840</v>
+        <v>31373</v>
       </c>
       <c r="G6" t="n">
-        <v>54810</v>
+        <v>47499</v>
       </c>
     </row>
     <row r="7">
@@ -585,22 +585,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="C7" t="n">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="D7" t="n">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E7" t="n">
-        <v>532</v>
+        <v>269</v>
       </c>
       <c r="F7" t="n">
-        <v>25696</v>
+        <v>33696</v>
       </c>
       <c r="G7" t="n">
-        <v>48412</v>
+        <v>47882</v>
       </c>
     </row>
     <row r="8">
@@ -608,22 +608,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C8" t="n">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="D8" t="n">
-        <v>179</v>
+        <v>309</v>
       </c>
       <c r="E8" t="n">
-        <v>427</v>
+        <v>339</v>
       </c>
       <c r="F8" t="n">
-        <v>27924</v>
+        <v>31827</v>
       </c>
       <c r="G8" t="n">
-        <v>50813</v>
+        <v>48477</v>
       </c>
     </row>
     <row r="9">
@@ -631,22 +631,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>110</v>
+        <v>206</v>
       </c>
       <c r="C9" t="n">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="D9" t="n">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="E9" t="n">
-        <v>382</v>
+        <v>467</v>
       </c>
       <c r="F9" t="n">
-        <v>27984</v>
+        <v>30821</v>
       </c>
       <c r="G9" t="n">
-        <v>50806</v>
+        <v>37827</v>
       </c>
     </row>
     <row r="10">
@@ -654,22 +654,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="C10" t="n">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D10" t="n">
-        <v>264</v>
+        <v>164</v>
       </c>
       <c r="E10" t="n">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="F10" t="n">
-        <v>28512</v>
+        <v>33620</v>
       </c>
       <c r="G10" t="n">
-        <v>51230</v>
+        <v>37700</v>
       </c>
     </row>
     <row r="11">
@@ -677,22 +677,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="C11" t="n">
-        <v>216</v>
+        <v>247</v>
       </c>
       <c r="D11" t="n">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E11" t="n">
-        <v>481</v>
+        <v>369</v>
       </c>
       <c r="F11" t="n">
-        <v>29315</v>
+        <v>36036</v>
       </c>
       <c r="G11" t="n">
-        <v>55315</v>
+        <v>38007</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="C12" t="n">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="D12" t="n">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="E12" t="n">
-        <v>271</v>
+        <v>161</v>
       </c>
       <c r="F12" t="n">
-        <v>26680</v>
+        <v>38380</v>
       </c>
       <c r="G12" t="n">
-        <v>58265</v>
+        <v>39767</v>
       </c>
     </row>
     <row r="13">
@@ -723,22 +723,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>230</v>
+        <v>124</v>
       </c>
       <c r="C13" t="n">
-        <v>205</v>
+        <v>103</v>
       </c>
       <c r="D13" t="n">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="E13" t="n">
-        <v>280</v>
+        <v>224</v>
       </c>
       <c r="F13" t="n">
-        <v>27430</v>
+        <v>41693</v>
       </c>
       <c r="G13" t="n">
-        <v>61320</v>
+        <v>42784</v>
       </c>
     </row>
     <row r="14">
@@ -746,22 +746,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="C14" t="n">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="D14" t="n">
-        <v>128</v>
+        <v>336</v>
       </c>
       <c r="E14" t="n">
-        <v>305</v>
+        <v>452</v>
       </c>
       <c r="F14" t="n">
-        <v>26368</v>
+        <v>38640</v>
       </c>
       <c r="G14" t="n">
-        <v>50630</v>
+        <v>41132</v>
       </c>
     </row>
     <row r="15">
@@ -769,22 +769,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="C15" t="n">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="D15" t="n">
-        <v>156</v>
+        <v>289</v>
       </c>
       <c r="E15" t="n">
-        <v>290</v>
+        <v>197</v>
       </c>
       <c r="F15" t="n">
-        <v>28080</v>
+        <v>41038</v>
       </c>
       <c r="G15" t="n">
-        <v>50460</v>
+        <v>40976</v>
       </c>
     </row>
     <row r="16">
@@ -792,22 +792,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C16" t="n">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D16" t="n">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="E16" t="n">
-        <v>319</v>
+        <v>381</v>
       </c>
       <c r="F16" t="n">
-        <v>28290</v>
+        <v>44775</v>
       </c>
       <c r="G16" t="n">
-        <v>52954</v>
+        <v>43434</v>
       </c>
     </row>
     <row r="17">
@@ -815,22 +815,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>178</v>
+        <v>226</v>
       </c>
       <c r="C17" t="n">
-        <v>110</v>
+        <v>234</v>
       </c>
       <c r="D17" t="n">
-        <v>217</v>
+        <v>427</v>
       </c>
       <c r="E17" t="n">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="F17" t="n">
-        <v>26691</v>
+        <v>46543</v>
       </c>
       <c r="G17" t="n">
-        <v>52920</v>
+        <v>42174</v>
       </c>
     </row>
     <row r="18">
@@ -838,22 +838,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="C18" t="n">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="D18" t="n">
-        <v>151</v>
+        <v>212</v>
       </c>
       <c r="E18" t="n">
-        <v>495</v>
+        <v>194</v>
       </c>
       <c r="F18" t="n">
-        <v>26878</v>
+        <v>40492</v>
       </c>
       <c r="G18" t="n">
-        <v>54450</v>
+        <v>42292</v>
       </c>
     </row>
     <row r="19">
@@ -861,22 +861,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="C19" t="n">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="D19" t="n">
-        <v>137</v>
+        <v>251</v>
       </c>
       <c r="E19" t="n">
-        <v>385</v>
+        <v>226</v>
       </c>
       <c r="F19" t="n">
-        <v>24523</v>
+        <v>39658</v>
       </c>
       <c r="G19" t="n">
-        <v>46200</v>
+        <v>41132</v>
       </c>
     </row>
     <row r="20">
@@ -884,22 +884,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="C20" t="n">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="D20" t="n">
-        <v>120</v>
+        <v>183</v>
       </c>
       <c r="E20" t="n">
-        <v>320</v>
+        <v>224</v>
       </c>
       <c r="F20" t="n">
-        <v>24720</v>
+        <v>43005</v>
       </c>
       <c r="G20" t="n">
-        <v>48960</v>
+        <v>43904</v>
       </c>
     </row>
     <row r="21">
@@ -907,22 +907,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>116</v>
+        <v>238</v>
       </c>
       <c r="C21" t="n">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="D21" t="n">
-        <v>198</v>
+        <v>414</v>
       </c>
       <c r="E21" t="n">
-        <v>431</v>
+        <v>186</v>
       </c>
       <c r="F21" t="n">
-        <v>27126</v>
+        <v>39330</v>
       </c>
       <c r="G21" t="n">
-        <v>50427</v>
+        <v>44640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se ajustan los gráficos: auto ajustables
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,13 +470,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>167</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>162</v>
+        <v>40</v>
       </c>
       <c r="D2" t="n">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="E2" t="n">
         <v>1000</v>
@@ -493,22 +493,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>232</v>
+        <v>37</v>
       </c>
       <c r="C3" t="n">
-        <v>172</v>
+        <v>47</v>
       </c>
       <c r="D3" t="n">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="E3" t="n">
         <v>1000</v>
       </c>
       <c r="F3" t="n">
-        <v>27000</v>
+        <v>7200</v>
       </c>
       <c r="G3" t="n">
-        <v>46000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="4">
@@ -516,22 +516,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
-        <v>230</v>
+        <v>43</v>
       </c>
       <c r="D4" t="n">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="E4" t="n">
-        <v>267</v>
+        <v>351</v>
       </c>
       <c r="F4" t="n">
-        <v>28536</v>
+        <v>6592</v>
       </c>
       <c r="G4" t="n">
-        <v>45924</v>
+        <v>11934</v>
       </c>
     </row>
     <row r="5">
@@ -539,22 +539,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>233</v>
+        <v>40</v>
       </c>
       <c r="C5" t="n">
-        <v>223</v>
+        <v>33</v>
       </c>
       <c r="D5" t="n">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E5" t="n">
-        <v>211</v>
+        <v>305</v>
       </c>
       <c r="F5" t="n">
-        <v>29670</v>
+        <v>6350</v>
       </c>
       <c r="G5" t="n">
-        <v>46631</v>
+        <v>12505</v>
       </c>
     </row>
     <row r="6">
@@ -562,22 +562,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>235</v>
+        <v>46</v>
       </c>
       <c r="C6" t="n">
-        <v>178</v>
+        <v>23</v>
       </c>
       <c r="D6" t="n">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="E6" t="n">
-        <v>213</v>
+        <v>390</v>
       </c>
       <c r="F6" t="n">
-        <v>31373</v>
+        <v>6142</v>
       </c>
       <c r="G6" t="n">
-        <v>47499</v>
+        <v>10140</v>
       </c>
     </row>
     <row r="7">
@@ -585,22 +585,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>144</v>
+        <v>47</v>
       </c>
       <c r="D7" t="n">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E7" t="n">
-        <v>269</v>
+        <v>471</v>
       </c>
       <c r="F7" t="n">
-        <v>33696</v>
+        <v>5945</v>
       </c>
       <c r="G7" t="n">
-        <v>47882</v>
+        <v>3297</v>
       </c>
     </row>
     <row r="8">
@@ -608,22 +608,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="C8" t="n">
-        <v>112</v>
+        <v>43</v>
       </c>
       <c r="D8" t="n">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="E8" t="n">
-        <v>339</v>
+        <v>71</v>
       </c>
       <c r="F8" t="n">
-        <v>31827</v>
+        <v>6111</v>
       </c>
       <c r="G8" t="n">
-        <v>48477</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="9">
@@ -631,22 +631,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>206</v>
+        <v>37</v>
       </c>
       <c r="C9" t="n">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="D9" t="n">
-        <v>259</v>
+        <v>144</v>
       </c>
       <c r="E9" t="n">
-        <v>467</v>
+        <v>83</v>
       </c>
       <c r="F9" t="n">
-        <v>30821</v>
+        <v>6624</v>
       </c>
       <c r="G9" t="n">
-        <v>37827</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="10">
@@ -654,22 +654,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>183</v>
+        <v>23</v>
       </c>
       <c r="C10" t="n">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="D10" t="n">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="E10" t="n">
-        <v>260</v>
+        <v>88</v>
       </c>
       <c r="F10" t="n">
-        <v>33620</v>
+        <v>6734</v>
       </c>
       <c r="G10" t="n">
-        <v>37700</v>
+        <v>3872</v>
       </c>
     </row>
     <row r="11">
@@ -677,22 +677,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>190</v>
+        <v>28</v>
       </c>
       <c r="C11" t="n">
-        <v>247</v>
+        <v>50</v>
       </c>
       <c r="D11" t="n">
-        <v>198</v>
+        <v>304</v>
       </c>
       <c r="E11" t="n">
-        <v>369</v>
+        <v>166</v>
       </c>
       <c r="F11" t="n">
-        <v>36036</v>
+        <v>6992</v>
       </c>
       <c r="G11" t="n">
-        <v>38007</v>
+        <v>3984</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>244</v>
+        <v>46</v>
       </c>
       <c r="C12" t="n">
-        <v>191</v>
+        <v>28</v>
       </c>
       <c r="D12" t="n">
-        <v>202</v>
+        <v>252</v>
       </c>
       <c r="E12" t="n">
-        <v>161</v>
+        <v>80</v>
       </c>
       <c r="F12" t="n">
-        <v>38380</v>
+        <v>6300</v>
       </c>
       <c r="G12" t="n">
-        <v>39767</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="13">
@@ -723,22 +723,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>124</v>
+        <v>28</v>
       </c>
       <c r="C13" t="n">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="D13" t="n">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="E13" t="n">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="F13" t="n">
-        <v>41693</v>
+        <v>6435</v>
       </c>
       <c r="G13" t="n">
-        <v>42784</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="14">
@@ -746,22 +746,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="C14" t="n">
-        <v>208</v>
+        <v>21</v>
       </c>
       <c r="D14" t="n">
-        <v>336</v>
+        <v>250</v>
       </c>
       <c r="E14" t="n">
-        <v>452</v>
+        <v>89</v>
       </c>
       <c r="F14" t="n">
-        <v>38640</v>
+        <v>6750</v>
       </c>
       <c r="G14" t="n">
-        <v>41132</v>
+        <v>4361</v>
       </c>
     </row>
     <row r="15">
@@ -769,22 +769,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>200</v>
+        <v>41</v>
       </c>
       <c r="C15" t="n">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="D15" t="n">
-        <v>289</v>
+        <v>171</v>
       </c>
       <c r="E15" t="n">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="F15" t="n">
-        <v>41038</v>
+        <v>7182</v>
       </c>
       <c r="G15" t="n">
-        <v>40976</v>
+        <v>4704</v>
       </c>
     </row>
     <row r="16">
@@ -792,22 +792,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="C16" t="n">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="D16" t="n">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="E16" t="n">
-        <v>381</v>
+        <v>179</v>
       </c>
       <c r="F16" t="n">
-        <v>44775</v>
+        <v>7410</v>
       </c>
       <c r="G16" t="n">
-        <v>43434</v>
+        <v>4654</v>
       </c>
     </row>
     <row r="17">
@@ -815,22 +815,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
+        <v>30</v>
+      </c>
+      <c r="C17" t="n">
+        <v>32</v>
+      </c>
+      <c r="D17" t="n">
         <v>226</v>
       </c>
-      <c r="C17" t="n">
-        <v>234</v>
-      </c>
-      <c r="D17" t="n">
-        <v>427</v>
-      </c>
       <c r="E17" t="n">
-        <v>426</v>
+        <v>172</v>
       </c>
       <c r="F17" t="n">
-        <v>46543</v>
+        <v>7458</v>
       </c>
       <c r="G17" t="n">
-        <v>42174</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="18">
@@ -838,22 +838,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>177</v>
+        <v>20</v>
       </c>
       <c r="C18" t="n">
-        <v>189</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>212</v>
+        <v>258</v>
       </c>
       <c r="E18" t="n">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="F18" t="n">
-        <v>40492</v>
+        <v>6450</v>
       </c>
       <c r="G18" t="n">
-        <v>42292</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="19">
@@ -861,22 +861,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>238</v>
+        <v>31</v>
       </c>
       <c r="C19" t="n">
-        <v>198</v>
+        <v>40</v>
       </c>
       <c r="D19" t="n">
-        <v>251</v>
+        <v>351</v>
       </c>
       <c r="E19" t="n">
-        <v>226</v>
+        <v>150</v>
       </c>
       <c r="F19" t="n">
-        <v>39658</v>
+        <v>6318</v>
       </c>
       <c r="G19" t="n">
-        <v>41132</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="20">
@@ -884,22 +884,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="C20" t="n">
-        <v>240</v>
+        <v>27</v>
       </c>
       <c r="D20" t="n">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="E20" t="n">
-        <v>224</v>
+        <v>109</v>
       </c>
       <c r="F20" t="n">
-        <v>43005</v>
+        <v>6540</v>
       </c>
       <c r="G20" t="n">
-        <v>43904</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="21">
@@ -907,22 +907,712 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
+        <v>43</v>
+      </c>
+      <c r="C21" t="n">
+        <v>23</v>
+      </c>
+      <c r="D21" t="n">
+        <v>321</v>
+      </c>
+      <c r="E21" t="n">
+        <v>174</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5778</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>28</v>
+      </c>
+      <c r="C22" t="n">
+        <v>42</v>
+      </c>
+      <c r="D22" t="n">
+        <v>142</v>
+      </c>
+      <c r="E22" t="n">
+        <v>204</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5964</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4488</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" t="n">
+        <v>48</v>
+      </c>
+      <c r="D23" t="n">
+        <v>227</v>
+      </c>
+      <c r="E23" t="n">
+        <v>110</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5902</v>
+      </c>
+      <c r="G23" t="n">
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>38</v>
+      </c>
+      <c r="C24" t="n">
+        <v>26</v>
+      </c>
+      <c r="D24" t="n">
+        <v>283</v>
+      </c>
+      <c r="E24" t="n">
+        <v>92</v>
+      </c>
+      <c r="F24" t="n">
+        <v>5377</v>
+      </c>
+      <c r="G24" t="n">
+        <v>4324</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>36</v>
+      </c>
+      <c r="C25" t="n">
+        <v>37</v>
+      </c>
+      <c r="D25" t="n">
+        <v>144</v>
+      </c>
+      <c r="E25" t="n">
+        <v>181</v>
+      </c>
+      <c r="F25" t="n">
+        <v>5472</v>
+      </c>
+      <c r="G25" t="n">
+        <v>4706</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>26</v>
+      </c>
+      <c r="C26" t="n">
+        <v>48</v>
+      </c>
+      <c r="D26" t="n">
+        <v>155</v>
+      </c>
+      <c r="E26" t="n">
+        <v>139</v>
+      </c>
+      <c r="F26" t="n">
+        <v>5580</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5143</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>36</v>
+      </c>
+      <c r="C27" t="n">
+        <v>36</v>
+      </c>
+      <c r="D27" t="n">
+        <v>227</v>
+      </c>
+      <c r="E27" t="n">
+        <v>115</v>
+      </c>
+      <c r="F27" t="n">
+        <v>5221</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>32</v>
+      </c>
+      <c r="C28" t="n">
+        <v>28</v>
+      </c>
+      <c r="D28" t="n">
+        <v>153</v>
+      </c>
+      <c r="E28" t="n">
+        <v>165</v>
+      </c>
+      <c r="F28" t="n">
+        <v>5355</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5940</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>25</v>
+      </c>
+      <c r="C29" t="n">
+        <v>46</v>
+      </c>
+      <c r="D29" t="n">
+        <v>175</v>
+      </c>
+      <c r="E29" t="n">
+        <v>233</v>
+      </c>
+      <c r="F29" t="n">
+        <v>5600</v>
+      </c>
+      <c r="G29" t="n">
+        <v>6524</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>32</v>
+      </c>
+      <c r="C30" t="n">
+        <v>43</v>
+      </c>
+      <c r="D30" t="n">
+        <v>224</v>
+      </c>
+      <c r="E30" t="n">
+        <v>150</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5600</v>
+      </c>
+      <c r="G30" t="n">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>40</v>
+      </c>
+      <c r="C31" t="n">
+        <v>32</v>
+      </c>
+      <c r="D31" t="n">
+        <v>190</v>
+      </c>
+      <c r="E31" t="n">
+        <v>163</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6080</v>
+      </c>
+      <c r="G31" t="n">
+        <v>6683</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>22</v>
+      </c>
+      <c r="C32" t="n">
+        <v>22</v>
+      </c>
+      <c r="D32" t="n">
+        <v>155</v>
+      </c>
+      <c r="E32" t="n">
+        <v>225</v>
+      </c>
+      <c r="F32" t="n">
+        <v>6200</v>
+      </c>
+      <c r="G32" t="n">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>27</v>
+      </c>
+      <c r="C33" t="n">
+        <v>29</v>
+      </c>
+      <c r="D33" t="n">
+        <v>290</v>
+      </c>
+      <c r="E33" t="n">
+        <v>343</v>
+      </c>
+      <c r="F33" t="n">
+        <v>6380</v>
+      </c>
+      <c r="G33" t="n">
+        <v>7546</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>42</v>
+      </c>
+      <c r="C34" t="n">
+        <v>28</v>
+      </c>
+      <c r="D34" t="n">
         <v>238</v>
       </c>
-      <c r="C21" t="n">
-        <v>119</v>
-      </c>
-      <c r="D21" t="n">
-        <v>414</v>
-      </c>
-      <c r="E21" t="n">
-        <v>186</v>
-      </c>
-      <c r="F21" t="n">
-        <v>39330</v>
-      </c>
-      <c r="G21" t="n">
-        <v>44640</v>
+      <c r="E34" t="n">
+        <v>268</v>
+      </c>
+      <c r="F34" t="n">
+        <v>5712</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7236</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>46</v>
+      </c>
+      <c r="C35" t="n">
+        <v>44</v>
+      </c>
+      <c r="D35" t="n">
+        <v>138</v>
+      </c>
+      <c r="E35" t="n">
+        <v>276</v>
+      </c>
+      <c r="F35" t="n">
+        <v>5796</v>
+      </c>
+      <c r="G35" t="n">
+        <v>7452</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>23</v>
+      </c>
+      <c r="C36" t="n">
+        <v>41</v>
+      </c>
+      <c r="D36" t="n">
+        <v>133</v>
+      </c>
+      <c r="E36" t="n">
+        <v>174</v>
+      </c>
+      <c r="F36" t="n">
+        <v>5985</v>
+      </c>
+      <c r="G36" t="n">
+        <v>7482</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="n">
+        <v>25</v>
+      </c>
+      <c r="D37" t="n">
+        <v>268</v>
+      </c>
+      <c r="E37" t="n">
+        <v>191</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4824</v>
+      </c>
+      <c r="G37" t="n">
+        <v>7640</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>30</v>
+      </c>
+      <c r="C38" t="n">
+        <v>44</v>
+      </c>
+      <c r="D38" t="n">
+        <v>139</v>
+      </c>
+      <c r="E38" t="n">
+        <v>311</v>
+      </c>
+      <c r="F38" t="n">
+        <v>5004</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6531</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>34</v>
+      </c>
+      <c r="C39" t="n">
+        <v>42</v>
+      </c>
+      <c r="D39" t="n">
+        <v>166</v>
+      </c>
+      <c r="E39" t="n">
+        <v>151</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4648</v>
+      </c>
+      <c r="G39" t="n">
+        <v>6342</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>36</v>
+      </c>
+      <c r="C40" t="n">
+        <v>45</v>
+      </c>
+      <c r="D40" t="n">
+        <v>149</v>
+      </c>
+      <c r="E40" t="n">
+        <v>157</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4917</v>
+      </c>
+      <c r="G40" t="n">
+        <v>6594</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" t="n">
+        <v>41</v>
+      </c>
+      <c r="D41" t="n">
+        <v>144</v>
+      </c>
+      <c r="E41" t="n">
+        <v>159</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4176</v>
+      </c>
+      <c r="G41" t="n">
+        <v>7155</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>29</v>
+      </c>
+      <c r="C42" t="n">
+        <v>44</v>
+      </c>
+      <c r="D42" t="n">
+        <v>105</v>
+      </c>
+      <c r="E42" t="n">
+        <v>174</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4200</v>
+      </c>
+      <c r="G42" t="n">
+        <v>7134</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>49</v>
+      </c>
+      <c r="C43" t="n">
+        <v>38</v>
+      </c>
+      <c r="D43" t="n">
+        <v>150</v>
+      </c>
+      <c r="E43" t="n">
+        <v>168</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4350</v>
+      </c>
+      <c r="G43" t="n">
+        <v>7392</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>32</v>
+      </c>
+      <c r="C44" t="n">
+        <v>39</v>
+      </c>
+      <c r="D44" t="n">
+        <v>89</v>
+      </c>
+      <c r="E44" t="n">
+        <v>212</v>
+      </c>
+      <c r="F44" t="n">
+        <v>4361</v>
+      </c>
+      <c r="G44" t="n">
+        <v>7420</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>45</v>
+      </c>
+      <c r="C45" t="n">
+        <v>43</v>
+      </c>
+      <c r="D45" t="n">
+        <v>144</v>
+      </c>
+      <c r="E45" t="n">
+        <v>190</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2304</v>
+      </c>
+      <c r="G45" t="n">
+        <v>6270</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>32</v>
+      </c>
+      <c r="C46" t="n">
+        <v>23</v>
+      </c>
+      <c r="D46" t="n">
+        <v>52</v>
+      </c>
+      <c r="E46" t="n">
+        <v>151</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2288</v>
+      </c>
+      <c r="G46" t="n">
+        <v>6040</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>41</v>
+      </c>
+      <c r="C47" t="n">
+        <v>46</v>
+      </c>
+      <c r="D47" t="n">
+        <v>78</v>
+      </c>
+      <c r="E47" t="n">
+        <v>283</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2496</v>
+      </c>
+      <c r="G47" t="n">
+        <v>6509</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>25</v>
+      </c>
+      <c r="C48" t="n">
+        <v>44</v>
+      </c>
+      <c r="D48" t="n">
+        <v>66</v>
+      </c>
+      <c r="E48" t="n">
+        <v>147</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2706</v>
+      </c>
+      <c r="G48" t="n">
+        <v>6762</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>20</v>
+      </c>
+      <c r="C49" t="n">
+        <v>46</v>
+      </c>
+      <c r="D49" t="n">
+        <v>110</v>
+      </c>
+      <c r="E49" t="n">
+        <v>153</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2640</v>
+      </c>
+      <c r="G49" t="n">
+        <v>6732</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>41</v>
+      </c>
+      <c r="C50" t="n">
+        <v>20</v>
+      </c>
+      <c r="D50" t="n">
+        <v>139</v>
+      </c>
+      <c r="E50" t="n">
+        <v>153</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2502</v>
+      </c>
+      <c r="G50" t="n">
+        <v>6579</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>33</v>
+      </c>
+      <c r="C51" t="n">
+        <v>47</v>
+      </c>
+      <c r="D51" t="n">
+        <v>65</v>
+      </c>
+      <c r="E51" t="n">
+        <v>351</v>
+      </c>
+      <c r="F51" t="n">
+        <v>2535</v>
+      </c>
+      <c r="G51" t="n">
+        <v>6669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se Finalizan actualizaciones - By Carjes
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -470,16 +470,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>313</v>
       </c>
       <c r="C2" t="n">
-        <v>40</v>
+        <v>313</v>
       </c>
       <c r="D2" t="n">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="E2" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -493,22 +493,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>37</v>
+        <v>397</v>
       </c>
       <c r="C3" t="n">
-        <v>47</v>
+        <v>467</v>
       </c>
       <c r="D3" t="n">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="E3" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="F3" t="n">
-        <v>7200</v>
+        <v>75900</v>
       </c>
       <c r="G3" t="n">
-        <v>15000</v>
+        <v>84600</v>
       </c>
     </row>
     <row r="4">
@@ -516,22 +516,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>28</v>
+        <v>279</v>
       </c>
       <c r="C4" t="n">
-        <v>43</v>
+        <v>494</v>
       </c>
       <c r="D4" t="n">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E4" t="n">
-        <v>351</v>
+        <v>200</v>
       </c>
       <c r="F4" t="n">
-        <v>6592</v>
+        <v>79400</v>
       </c>
       <c r="G4" t="n">
-        <v>11934</v>
+        <v>93400</v>
       </c>
     </row>
     <row r="5">
@@ -539,22 +539,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>40</v>
+        <v>406</v>
       </c>
       <c r="C5" t="n">
-        <v>33</v>
+        <v>485</v>
       </c>
       <c r="D5" t="n">
-        <v>254</v>
+        <v>400</v>
       </c>
       <c r="E5" t="n">
-        <v>305</v>
+        <v>400</v>
       </c>
       <c r="F5" t="n">
-        <v>6350</v>
+        <v>111600</v>
       </c>
       <c r="G5" t="n">
-        <v>12505</v>
+        <v>197600</v>
       </c>
     </row>
     <row r="6">
@@ -562,22 +562,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>46</v>
+        <v>579</v>
       </c>
       <c r="C6" t="n">
-        <v>23</v>
+        <v>668</v>
       </c>
       <c r="D6" t="n">
-        <v>166</v>
+        <v>800</v>
       </c>
       <c r="E6" t="n">
-        <v>390</v>
+        <v>800</v>
       </c>
       <c r="F6" t="n">
-        <v>6142</v>
+        <v>148800</v>
       </c>
       <c r="G6" t="n">
-        <v>10140</v>
+        <v>187200</v>
       </c>
     </row>
     <row r="7">
@@ -585,22 +585,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>21</v>
+        <v>423</v>
       </c>
       <c r="C7" t="n">
-        <v>47</v>
+        <v>243</v>
       </c>
       <c r="D7" t="n">
-        <v>145</v>
+        <v>200</v>
       </c>
       <c r="E7" t="n">
-        <v>471</v>
+        <v>300</v>
       </c>
       <c r="F7" t="n">
-        <v>5945</v>
+        <v>115800</v>
       </c>
       <c r="G7" t="n">
-        <v>3297</v>
+        <v>200400</v>
       </c>
     </row>
     <row r="8">
@@ -608,22 +608,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>46</v>
+        <v>404</v>
       </c>
       <c r="C8" t="n">
-        <v>43</v>
+        <v>320</v>
       </c>
       <c r="D8" t="n">
-        <v>291</v>
+        <v>400</v>
       </c>
       <c r="E8" t="n">
-        <v>71</v>
+        <v>600</v>
       </c>
       <c r="F8" t="n">
-        <v>6111</v>
+        <v>169200</v>
       </c>
       <c r="G8" t="n">
-        <v>3337</v>
+        <v>145800</v>
       </c>
     </row>
     <row r="9">
@@ -631,22 +631,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>37</v>
+        <v>436</v>
       </c>
       <c r="C9" t="n">
-        <v>44</v>
+        <v>647</v>
       </c>
       <c r="D9" t="n">
-        <v>144</v>
+        <v>800</v>
       </c>
       <c r="E9" t="n">
-        <v>83</v>
+        <v>1200</v>
       </c>
       <c r="F9" t="n">
-        <v>6624</v>
+        <v>227200</v>
       </c>
       <c r="G9" t="n">
-        <v>3569</v>
+        <v>126000</v>
       </c>
     </row>
     <row r="10">
@@ -654,22 +654,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>23</v>
+        <v>267</v>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>444</v>
       </c>
       <c r="D10" t="n">
-        <v>182</v>
+        <v>300</v>
       </c>
       <c r="E10" t="n">
-        <v>88</v>
+        <v>300</v>
       </c>
       <c r="F10" t="n">
-        <v>6734</v>
+        <v>130800</v>
       </c>
       <c r="G10" t="n">
-        <v>3872</v>
+        <v>194100</v>
       </c>
     </row>
     <row r="11">
@@ -677,22 +677,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>28</v>
+        <v>461</v>
       </c>
       <c r="C11" t="n">
-        <v>50</v>
+        <v>287</v>
       </c>
       <c r="D11" t="n">
-        <v>304</v>
+        <v>600</v>
       </c>
       <c r="E11" t="n">
-        <v>166</v>
+        <v>600</v>
       </c>
       <c r="F11" t="n">
-        <v>6992</v>
+        <v>145200</v>
       </c>
       <c r="G11" t="n">
-        <v>3984</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>46</v>
+        <v>498</v>
       </c>
       <c r="C12" t="n">
-        <v>28</v>
+        <v>374</v>
       </c>
       <c r="D12" t="n">
-        <v>252</v>
+        <v>400</v>
       </c>
       <c r="E12" t="n">
-        <v>80</v>
+        <v>500</v>
       </c>
       <c r="F12" t="n">
-        <v>6300</v>
+        <v>184400</v>
       </c>
       <c r="G12" t="n">
-        <v>3920</v>
+        <v>143500</v>
       </c>
     </row>
     <row r="13">
@@ -723,22 +723,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>28</v>
+        <v>658</v>
       </c>
       <c r="C13" t="n">
-        <v>50</v>
+        <v>632</v>
       </c>
       <c r="D13" t="n">
-        <v>143</v>
+        <v>800</v>
       </c>
       <c r="E13" t="n">
-        <v>152</v>
+        <v>1000</v>
       </c>
       <c r="F13" t="n">
-        <v>6435</v>
+        <v>225600</v>
       </c>
       <c r="G13" t="n">
-        <v>4256</v>
+        <v>149000</v>
       </c>
     </row>
     <row r="14">
@@ -746,22 +746,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>43</v>
+        <v>331</v>
       </c>
       <c r="C14" t="n">
-        <v>21</v>
+        <v>445</v>
       </c>
       <c r="D14" t="n">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="E14" t="n">
-        <v>89</v>
+        <v>400</v>
       </c>
       <c r="F14" t="n">
-        <v>6750</v>
+        <v>130200</v>
       </c>
       <c r="G14" t="n">
-        <v>4361</v>
+        <v>252800</v>
       </c>
     </row>
     <row r="15">
@@ -769,22 +769,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>41</v>
+        <v>595</v>
       </c>
       <c r="C15" t="n">
-        <v>28</v>
+        <v>682</v>
       </c>
       <c r="D15" t="n">
-        <v>171</v>
+        <v>700</v>
       </c>
       <c r="E15" t="n">
-        <v>224</v>
+        <v>800</v>
       </c>
       <c r="F15" t="n">
-        <v>7182</v>
+        <v>156800</v>
       </c>
       <c r="G15" t="n">
-        <v>4704</v>
+        <v>196000</v>
       </c>
     </row>
     <row r="16">
@@ -792,22 +792,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>36</v>
+        <v>479</v>
       </c>
       <c r="C16" t="n">
-        <v>28</v>
+        <v>445</v>
       </c>
       <c r="D16" t="n">
-        <v>190</v>
+        <v>300</v>
       </c>
       <c r="E16" t="n">
-        <v>179</v>
+        <v>300</v>
       </c>
       <c r="F16" t="n">
-        <v>7410</v>
+        <v>167100</v>
       </c>
       <c r="G16" t="n">
-        <v>4654</v>
+        <v>191100</v>
       </c>
     </row>
     <row r="17">
@@ -815,22 +815,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>30</v>
+        <v>373</v>
       </c>
       <c r="C17" t="n">
-        <v>32</v>
+        <v>445</v>
       </c>
       <c r="D17" t="n">
-        <v>226</v>
+        <v>500</v>
       </c>
       <c r="E17" t="n">
-        <v>172</v>
+        <v>400</v>
       </c>
       <c r="F17" t="n">
-        <v>7458</v>
+        <v>192000</v>
       </c>
       <c r="G17" t="n">
-        <v>4300</v>
+        <v>172400</v>
       </c>
     </row>
     <row r="18">
@@ -838,22 +838,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>20</v>
+        <v>327</v>
       </c>
       <c r="C18" t="n">
-        <v>30</v>
+        <v>480</v>
       </c>
       <c r="D18" t="n">
-        <v>258</v>
+        <v>500</v>
       </c>
       <c r="E18" t="n">
-        <v>143</v>
+        <v>600</v>
       </c>
       <c r="F18" t="n">
-        <v>6450</v>
+        <v>148500</v>
       </c>
       <c r="G18" t="n">
-        <v>4433</v>
+        <v>174600</v>
       </c>
     </row>
     <row r="19">
@@ -861,22 +861,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>31</v>
+        <v>379</v>
       </c>
       <c r="C19" t="n">
-        <v>40</v>
+        <v>549</v>
       </c>
       <c r="D19" t="n">
-        <v>351</v>
+        <v>600</v>
       </c>
       <c r="E19" t="n">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="F19" t="n">
-        <v>6318</v>
+        <v>114600</v>
       </c>
       <c r="G19" t="n">
-        <v>4350</v>
+        <v>172400</v>
       </c>
     </row>
     <row r="20">
@@ -884,22 +884,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>22</v>
+        <v>272</v>
       </c>
       <c r="C20" t="n">
-        <v>27</v>
+        <v>301</v>
       </c>
       <c r="D20" t="n">
-        <v>218</v>
+        <v>500</v>
       </c>
       <c r="E20" t="n">
-        <v>109</v>
+        <v>400</v>
       </c>
       <c r="F20" t="n">
-        <v>6540</v>
+        <v>157500</v>
       </c>
       <c r="G20" t="n">
-        <v>4360</v>
+        <v>206400</v>
       </c>
     </row>
     <row r="21">
@@ -907,22 +907,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>43</v>
+        <v>323</v>
       </c>
       <c r="C21" t="n">
-        <v>23</v>
+        <v>261</v>
       </c>
       <c r="D21" t="n">
-        <v>321</v>
+        <v>800</v>
       </c>
       <c r="E21" t="n">
-        <v>174</v>
+        <v>700</v>
       </c>
       <c r="F21" t="n">
-        <v>5778</v>
+        <v>138400</v>
       </c>
       <c r="G21" t="n">
-        <v>4698</v>
+        <v>174300</v>
       </c>
     </row>
     <row r="22">
@@ -930,22 +930,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>28</v>
+        <v>409</v>
       </c>
       <c r="C22" t="n">
-        <v>42</v>
+        <v>261</v>
       </c>
       <c r="D22" t="n">
-        <v>142</v>
+        <v>600</v>
       </c>
       <c r="E22" t="n">
-        <v>204</v>
+        <v>700</v>
       </c>
       <c r="F22" t="n">
-        <v>5964</v>
+        <v>172200</v>
       </c>
       <c r="G22" t="n">
-        <v>4488</v>
+        <v>151200</v>
       </c>
     </row>
     <row r="23">
@@ -953,22 +953,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>21</v>
+        <v>398</v>
       </c>
       <c r="C23" t="n">
-        <v>48</v>
+        <v>411</v>
       </c>
       <c r="D23" t="n">
-        <v>227</v>
+        <v>500</v>
       </c>
       <c r="E23" t="n">
-        <v>110</v>
+        <v>700</v>
       </c>
       <c r="F23" t="n">
-        <v>5902</v>
+        <v>202000</v>
       </c>
       <c r="G23" t="n">
-        <v>4290</v>
+        <v>178500</v>
       </c>
     </row>
     <row r="24">
@@ -976,22 +976,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>38</v>
+        <v>286</v>
       </c>
       <c r="C24" t="n">
-        <v>26</v>
+        <v>530</v>
       </c>
       <c r="D24" t="n">
-        <v>283</v>
+        <v>500</v>
       </c>
       <c r="E24" t="n">
-        <v>92</v>
+        <v>700</v>
       </c>
       <c r="F24" t="n">
-        <v>5377</v>
+        <v>173500</v>
       </c>
       <c r="G24" t="n">
-        <v>4324</v>
+        <v>163100</v>
       </c>
     </row>
     <row r="25">
@@ -999,22 +999,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>36</v>
+        <v>300</v>
       </c>
       <c r="C25" t="n">
-        <v>37</v>
+        <v>469</v>
       </c>
       <c r="D25" t="n">
-        <v>144</v>
+        <v>600</v>
       </c>
       <c r="E25" t="n">
-        <v>181</v>
+        <v>400</v>
       </c>
       <c r="F25" t="n">
-        <v>5472</v>
+        <v>151800</v>
       </c>
       <c r="G25" t="n">
-        <v>4706</v>
+        <v>195200</v>
       </c>
     </row>
     <row r="26">
@@ -1022,22 +1022,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>26</v>
+        <v>459</v>
       </c>
       <c r="C26" t="n">
-        <v>48</v>
+        <v>431</v>
       </c>
       <c r="D26" t="n">
-        <v>155</v>
+        <v>800</v>
       </c>
       <c r="E26" t="n">
-        <v>139</v>
+        <v>500</v>
       </c>
       <c r="F26" t="n">
-        <v>5580</v>
+        <v>141600</v>
       </c>
       <c r="G26" t="n">
-        <v>5143</v>
+        <v>185000</v>
       </c>
     </row>
     <row r="27">
@@ -1045,22 +1045,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>36</v>
+        <v>282</v>
       </c>
       <c r="C27" t="n">
-        <v>36</v>
+        <v>433</v>
       </c>
       <c r="D27" t="n">
-        <v>227</v>
+        <v>400</v>
       </c>
       <c r="E27" t="n">
-        <v>115</v>
+        <v>500</v>
       </c>
       <c r="F27" t="n">
-        <v>5221</v>
+        <v>164800</v>
       </c>
       <c r="G27" t="n">
-        <v>5520</v>
+        <v>157000</v>
       </c>
     </row>
     <row r="28">
@@ -1068,22 +1068,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>32</v>
+        <v>378</v>
       </c>
       <c r="C28" t="n">
-        <v>28</v>
+        <v>472</v>
       </c>
       <c r="D28" t="n">
-        <v>153</v>
+        <v>700</v>
       </c>
       <c r="E28" t="n">
-        <v>165</v>
+        <v>500</v>
       </c>
       <c r="F28" t="n">
-        <v>5355</v>
+        <v>161700</v>
       </c>
       <c r="G28" t="n">
-        <v>5940</v>
+        <v>191000</v>
       </c>
     </row>
     <row r="29">
@@ -1091,22 +1091,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>25</v>
+        <v>405</v>
       </c>
       <c r="C29" t="n">
-        <v>46</v>
+        <v>303</v>
       </c>
       <c r="D29" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="E29" t="n">
-        <v>233</v>
+        <v>500</v>
       </c>
       <c r="F29" t="n">
-        <v>5600</v>
+        <v>175500</v>
       </c>
       <c r="G29" t="n">
-        <v>6524</v>
+        <v>230500</v>
       </c>
     </row>
     <row r="30">
@@ -1114,22 +1114,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>32</v>
+        <v>633</v>
       </c>
       <c r="C30" t="n">
-        <v>43</v>
+        <v>507</v>
       </c>
       <c r="D30" t="n">
-        <v>224</v>
+        <v>600</v>
       </c>
       <c r="E30" t="n">
-        <v>150</v>
+        <v>800</v>
       </c>
       <c r="F30" t="n">
-        <v>5600</v>
+        <v>156000</v>
       </c>
       <c r="G30" t="n">
-        <v>6750</v>
+        <v>148800</v>
       </c>
     </row>
     <row r="31">
@@ -1137,22 +1137,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>40</v>
+        <v>301</v>
       </c>
       <c r="C31" t="n">
-        <v>32</v>
+        <v>591</v>
       </c>
       <c r="D31" t="n">
-        <v>190</v>
+        <v>300</v>
       </c>
       <c r="E31" t="n">
-        <v>163</v>
+        <v>500</v>
       </c>
       <c r="F31" t="n">
-        <v>6080</v>
+        <v>163200</v>
       </c>
       <c r="G31" t="n">
-        <v>6683</v>
+        <v>176500</v>
       </c>
     </row>
     <row r="32">
@@ -1160,22 +1160,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>22</v>
+        <v>493</v>
       </c>
       <c r="C32" t="n">
-        <v>22</v>
+        <v>459</v>
       </c>
       <c r="D32" t="n">
-        <v>155</v>
+        <v>600</v>
       </c>
       <c r="E32" t="n">
-        <v>225</v>
+        <v>400</v>
       </c>
       <c r="F32" t="n">
-        <v>6200</v>
+        <v>135000</v>
       </c>
       <c r="G32" t="n">
-        <v>7200</v>
+        <v>212800</v>
       </c>
     </row>
     <row r="33">
@@ -1183,22 +1183,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>27</v>
+        <v>618</v>
       </c>
       <c r="C33" t="n">
-        <v>29</v>
+        <v>399</v>
       </c>
       <c r="D33" t="n">
-        <v>290</v>
+        <v>400</v>
       </c>
       <c r="E33" t="n">
-        <v>343</v>
+        <v>500</v>
       </c>
       <c r="F33" t="n">
-        <v>6380</v>
+        <v>146800</v>
       </c>
       <c r="G33" t="n">
-        <v>7546</v>
+        <v>169500</v>
       </c>
     </row>
     <row r="34">
@@ -1206,22 +1206,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>42</v>
+        <v>237</v>
       </c>
       <c r="C34" t="n">
-        <v>28</v>
+        <v>396</v>
       </c>
       <c r="D34" t="n">
-        <v>238</v>
+        <v>300</v>
       </c>
       <c r="E34" t="n">
-        <v>268</v>
+        <v>500</v>
       </c>
       <c r="F34" t="n">
-        <v>5712</v>
+        <v>185400</v>
       </c>
       <c r="G34" t="n">
-        <v>7236</v>
+        <v>177500</v>
       </c>
     </row>
     <row r="35">
@@ -1229,22 +1229,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>46</v>
+        <v>284</v>
       </c>
       <c r="C35" t="n">
-        <v>44</v>
+        <v>240</v>
       </c>
       <c r="D35" t="n">
-        <v>138</v>
+        <v>600</v>
       </c>
       <c r="E35" t="n">
-        <v>276</v>
+        <v>600</v>
       </c>
       <c r="F35" t="n">
-        <v>5796</v>
+        <v>141000</v>
       </c>
       <c r="G35" t="n">
-        <v>7452</v>
+        <v>237600</v>
       </c>
     </row>
     <row r="36">
@@ -1252,22 +1252,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>23</v>
+        <v>369</v>
       </c>
       <c r="C36" t="n">
-        <v>41</v>
+        <v>624</v>
       </c>
       <c r="D36" t="n">
-        <v>133</v>
+        <v>1000</v>
       </c>
       <c r="E36" t="n">
-        <v>174</v>
+        <v>1200</v>
       </c>
       <c r="F36" t="n">
-        <v>5985</v>
+        <v>189000</v>
       </c>
       <c r="G36" t="n">
-        <v>7482</v>
+        <v>111600</v>
       </c>
     </row>
     <row r="37">
@@ -1275,22 +1275,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>36</v>
+        <v>409</v>
       </c>
       <c r="C37" t="n">
-        <v>25</v>
+        <v>358</v>
       </c>
       <c r="D37" t="n">
-        <v>268</v>
+        <v>400</v>
       </c>
       <c r="E37" t="n">
-        <v>191</v>
+        <v>400</v>
       </c>
       <c r="F37" t="n">
-        <v>4824</v>
+        <v>136400</v>
       </c>
       <c r="G37" t="n">
-        <v>7640</v>
+        <v>220800</v>
       </c>
     </row>
     <row r="38">
@@ -1298,22 +1298,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>30</v>
+        <v>313</v>
       </c>
       <c r="C38" t="n">
-        <v>44</v>
+        <v>428</v>
       </c>
       <c r="D38" t="n">
-        <v>139</v>
+        <v>700</v>
       </c>
       <c r="E38" t="n">
-        <v>311</v>
+        <v>400</v>
       </c>
       <c r="F38" t="n">
-        <v>5004</v>
+        <v>216300</v>
       </c>
       <c r="G38" t="n">
-        <v>6531</v>
+        <v>142400</v>
       </c>
     </row>
     <row r="39">
@@ -1321,22 +1321,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>34</v>
+        <v>219</v>
       </c>
       <c r="C39" t="n">
-        <v>42</v>
+        <v>467</v>
       </c>
       <c r="D39" t="n">
-        <v>166</v>
+        <v>400</v>
       </c>
       <c r="E39" t="n">
-        <v>151</v>
+        <v>800</v>
       </c>
       <c r="F39" t="n">
-        <v>4648</v>
+        <v>118000</v>
       </c>
       <c r="G39" t="n">
-        <v>6342</v>
+        <v>222400</v>
       </c>
     </row>
     <row r="40">
@@ -1344,22 +1344,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>36</v>
+        <v>395</v>
       </c>
       <c r="C40" t="n">
-        <v>45</v>
+        <v>471</v>
       </c>
       <c r="D40" t="n">
-        <v>149</v>
+        <v>1300</v>
       </c>
       <c r="E40" t="n">
-        <v>157</v>
+        <v>400</v>
       </c>
       <c r="F40" t="n">
-        <v>4917</v>
+        <v>120900</v>
       </c>
       <c r="G40" t="n">
-        <v>6594</v>
+        <v>186000</v>
       </c>
     </row>
     <row r="41">
@@ -1367,22 +1367,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>40</v>
+        <v>487</v>
       </c>
       <c r="C41" t="n">
-        <v>41</v>
+        <v>520</v>
       </c>
       <c r="D41" t="n">
-        <v>144</v>
+        <v>500</v>
       </c>
       <c r="E41" t="n">
-        <v>159</v>
+        <v>600</v>
       </c>
       <c r="F41" t="n">
-        <v>4176</v>
+        <v>152500</v>
       </c>
       <c r="G41" t="n">
-        <v>7155</v>
+        <v>186000</v>
       </c>
     </row>
     <row r="42">
@@ -1390,22 +1390,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>29</v>
+        <v>567</v>
       </c>
       <c r="C42" t="n">
-        <v>44</v>
+        <v>243</v>
       </c>
       <c r="D42" t="n">
-        <v>105</v>
+        <v>400</v>
       </c>
       <c r="E42" t="n">
-        <v>174</v>
+        <v>400</v>
       </c>
       <c r="F42" t="n">
-        <v>4200</v>
+        <v>154400</v>
       </c>
       <c r="G42" t="n">
-        <v>7134</v>
+        <v>201600</v>
       </c>
     </row>
     <row r="43">
@@ -1413,22 +1413,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>49</v>
+        <v>479</v>
       </c>
       <c r="C43" t="n">
-        <v>38</v>
+        <v>589</v>
       </c>
       <c r="D43" t="n">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="E43" t="n">
-        <v>168</v>
+        <v>1100</v>
       </c>
       <c r="F43" t="n">
-        <v>4350</v>
+        <v>222800</v>
       </c>
       <c r="G43" t="n">
-        <v>7392</v>
+        <v>154000</v>
       </c>
     </row>
     <row r="44">
@@ -1436,22 +1436,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>32</v>
+        <v>386</v>
       </c>
       <c r="C44" t="n">
-        <v>39</v>
+        <v>283</v>
       </c>
       <c r="D44" t="n">
-        <v>89</v>
+        <v>400</v>
       </c>
       <c r="E44" t="n">
-        <v>212</v>
+        <v>400</v>
       </c>
       <c r="F44" t="n">
-        <v>4361</v>
+        <v>165200</v>
       </c>
       <c r="G44" t="n">
-        <v>7420</v>
+        <v>213200</v>
       </c>
     </row>
     <row r="45">
@@ -1459,22 +1459,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>45</v>
+        <v>390</v>
       </c>
       <c r="C45" t="n">
-        <v>43</v>
+        <v>392</v>
       </c>
       <c r="D45" t="n">
-        <v>144</v>
+        <v>600</v>
       </c>
       <c r="E45" t="n">
-        <v>190</v>
+        <v>700</v>
       </c>
       <c r="F45" t="n">
-        <v>2304</v>
+        <v>211800</v>
       </c>
       <c r="G45" t="n">
-        <v>6270</v>
+        <v>142800</v>
       </c>
     </row>
     <row r="46">
@@ -1482,22 +1482,22 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>32</v>
+        <v>461</v>
       </c>
       <c r="C46" t="n">
-        <v>23</v>
+        <v>525</v>
       </c>
       <c r="D46" t="n">
-        <v>52</v>
+        <v>500</v>
       </c>
       <c r="E46" t="n">
-        <v>151</v>
+        <v>600</v>
       </c>
       <c r="F46" t="n">
-        <v>2288</v>
+        <v>170000</v>
       </c>
       <c r="G46" t="n">
-        <v>6040</v>
+        <v>212400</v>
       </c>
     </row>
     <row r="47">
@@ -1505,22 +1505,22 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>41</v>
+        <v>444</v>
       </c>
       <c r="C47" t="n">
-        <v>46</v>
+        <v>426</v>
       </c>
       <c r="D47" t="n">
-        <v>78</v>
+        <v>400</v>
       </c>
       <c r="E47" t="n">
-        <v>283</v>
+        <v>500</v>
       </c>
       <c r="F47" t="n">
-        <v>2496</v>
+        <v>134400</v>
       </c>
       <c r="G47" t="n">
-        <v>6509</v>
+        <v>176500</v>
       </c>
     </row>
     <row r="48">
@@ -1528,22 +1528,22 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>25</v>
+        <v>535</v>
       </c>
       <c r="C48" t="n">
-        <v>44</v>
+        <v>444</v>
       </c>
       <c r="D48" t="n">
-        <v>66</v>
+        <v>500</v>
       </c>
       <c r="E48" t="n">
-        <v>147</v>
+        <v>500</v>
       </c>
       <c r="F48" t="n">
-        <v>2706</v>
+        <v>160500</v>
       </c>
       <c r="G48" t="n">
-        <v>6762</v>
+        <v>158000</v>
       </c>
     </row>
     <row r="49">
@@ -1551,22 +1551,22 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>20</v>
+        <v>249</v>
       </c>
       <c r="C49" t="n">
-        <v>46</v>
+        <v>496</v>
       </c>
       <c r="D49" t="n">
-        <v>110</v>
+        <v>300</v>
       </c>
       <c r="E49" t="n">
-        <v>153</v>
+        <v>600</v>
       </c>
       <c r="F49" t="n">
-        <v>2640</v>
+        <v>147900</v>
       </c>
       <c r="G49" t="n">
-        <v>6732</v>
+        <v>205200</v>
       </c>
     </row>
     <row r="50">
@@ -1574,22 +1574,22 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>41</v>
+        <v>423</v>
       </c>
       <c r="C50" t="n">
-        <v>20</v>
+        <v>271</v>
       </c>
       <c r="D50" t="n">
-        <v>139</v>
+        <v>800</v>
       </c>
       <c r="E50" t="n">
-        <v>153</v>
+        <v>400</v>
       </c>
       <c r="F50" t="n">
-        <v>2502</v>
+        <v>134400</v>
       </c>
       <c r="G50" t="n">
-        <v>6579</v>
+        <v>194000</v>
       </c>
     </row>
     <row r="51">
@@ -1597,22 +1597,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>33</v>
+        <v>346</v>
       </c>
       <c r="C51" t="n">
-        <v>47</v>
+        <v>399</v>
       </c>
       <c r="D51" t="n">
-        <v>65</v>
+        <v>500</v>
       </c>
       <c r="E51" t="n">
-        <v>351</v>
+        <v>1000</v>
       </c>
       <c r="F51" t="n">
-        <v>2535</v>
+        <v>193000</v>
       </c>
       <c r="G51" t="n">
-        <v>6669</v>
+        <v>138000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>